<commit_message>
First version of scheduler and  some data
</commit_message>
<xml_diff>
--- a/recipes/white/White_wild_yeast_favorite.xlsx
+++ b/recipes/white/White_wild_yeast_favorite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="0" windowWidth="25040" windowHeight="17460" tabRatio="500" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="2020" yWindow="1260" windowWidth="23060" windowHeight="13440" tabRatio="500" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="GF_bakingMaguque_data" sheetId="10" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet name="gf_croissant_data" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet3" sheetId="9" r:id="rId8"/>
     <sheet name="Tartine_country_data" sheetId="11" r:id="rId9"/>
+    <sheet name="Napoleon" sheetId="12" r:id="rId10"/>
+    <sheet name="My_napoleon_recipe" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="180">
   <si>
     <t>bake</t>
   </si>
@@ -500,15 +502,9 @@
     <t>fed 8 hours before use</t>
   </si>
   <si>
-    <t>tartine country</t>
-  </si>
-  <si>
     <t>breadcalc.com, tartine country sourdough</t>
   </si>
   <si>
-    <t>350 bread, 100 AP, 40 whole wheat Whole Foods 365, 260 water, 80 whole wheat starter(100 hydration), 10 gr exxtra water, 11 g salt</t>
-  </si>
-  <si>
     <t>4 times, every 30 min, 2 hours</t>
   </si>
   <si>
@@ -534,6 +530,45 @@
   </si>
   <si>
     <t>whole wheat starter, 100 hydration, 10 hours rise</t>
+  </si>
+  <si>
+    <t>250 bread, 100 AP, 40 whole wheat Whole Foods 365, 260 water, 80 whole wheat starter(100 hydration), 10 gr exxtra water, 11 g salt</t>
+  </si>
+  <si>
+    <t>basic tartine country</t>
+  </si>
+  <si>
+    <t>very healthy rise</t>
+  </si>
+  <si>
+    <t>not very high oven spring, but very open crumb</t>
+  </si>
+  <si>
+    <t>autolyze from 9 am to 7 pm, S+F 3,5 hours, preshape and bench rest 30 min, proof overnight on open window,  bake 20 min 500F + 10 min 450 F</t>
+  </si>
+  <si>
+    <t>not high, looks like overproofed</t>
+  </si>
+  <si>
+    <t>autolyze 30 min, stretch and fold 2,5 hours, overnight cold fermentation, 30 min rest on table, shape, proof frm 9 to 3 70 F</t>
+  </si>
+  <si>
+    <t>room: 70+</t>
+  </si>
+  <si>
+    <t>I think the proof was long for 70 F and the dough was overproofed</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>puff pastry</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>packages</t>
   </si>
 </sst>
 </file>
@@ -546,6 +581,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -602,8 +638,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -653,7 +713,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -670,6 +730,18 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -686,6 +758,18 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1223,6 +1307,349 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="35" style="2" customWidth="1"/>
+    <col min="10" max="10" width="89.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="89.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="16" style="2" customWidth="1"/>
+    <col min="20" max="20" width="52.83203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="24.6640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="18.5" style="2" customWidth="1"/>
+    <col min="23" max="23" width="22.1640625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="5" customFormat="1" ht="168">
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="73" customHeight="1">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43421</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2" s="2">
+        <v>40</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>69</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="113" customHeight="1">
+      <c r="B3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43425</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>60</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="280">
+      <c r="B4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43425</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>70</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>70</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="C9" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
@@ -2891,21 +3318,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA3" sqref="AA3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="33.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="56.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="35" style="2" customWidth="1"/>
@@ -3007,7 +3431,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C2" s="3">
         <v>43421</v>
@@ -3016,22 +3440,25 @@
         <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="O2" s="2">
         <v>40</v>
@@ -3040,22 +3467,22 @@
         <v>70</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>79</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Y2" s="2">
         <v>69</v>
@@ -3064,14 +3491,90 @@
         <v>40</v>
       </c>
       <c r="AA2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="113" customHeight="1">
+      <c r="B3" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="113" customHeight="1">
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:27">
-      <c r="C4" s="3"/>
+      <c r="C3" s="3">
+        <v>43425</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>60</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="280">
+      <c r="B4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43425</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>70</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>70</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="5" spans="1:27">
       <c r="C5" s="3"/>

</xml_diff>

<commit_message>
yeast to dough converter
</commit_message>
<xml_diff>
--- a/recipes/white/White_wild_yeast_favorite.xlsx
+++ b/recipes/white/White_wild_yeast_favorite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="0" windowWidth="23680" windowHeight="14020" tabRatio="500"/>
+    <workbookView xWindow="2020" yWindow="0" windowWidth="23680" windowHeight="14020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GF_bakingMaguque_data" sheetId="10" r:id="rId1"/>
@@ -678,7 +678,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1230,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="W7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
@@ -1740,15 +1739,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
     <col min="5" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.5" style="1" bestFit="1" customWidth="1"/>

</xml_diff>